<commit_message>
Início Validação por Horário
</commit_message>
<xml_diff>
--- a/Arquivos/VARIÁVEIS E ARRAY.xlsx
+++ b/Arquivos/VARIÁVEIS E ARRAY.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e7075be29de02ca6/Documentos/Planilhas/YouTube/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prema\AppData\Roaming\MetaQuotes\Terminal\7B8FFB3E490B2B8923BCC10180ACB2DC\MQL5\Experts\Arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="136" documentId="8_{7F5068E3-0B2C-402E-AA38-8D4268AFCDE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2D038132-51A7-435B-85E0-A1CBD2066D05}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F9EB79-6192-4355-B462-1360907987AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{6F8BE7D0-2A52-4DE9-8F9D-E8FDF3F58D54}"/>
+    <workbookView xWindow="5190" yWindow="1545" windowWidth="20235" windowHeight="13215" activeTab="3" xr2:uid="{6F8BE7D0-2A52-4DE9-8F9D-E8FDF3F58D54}"/>
   </bookViews>
   <sheets>
     <sheet name="VARIÁVEIS" sheetId="4" r:id="rId1"/>
     <sheet name="ARRAY" sheetId="1" r:id="rId2"/>
     <sheet name="DADOS" sheetId="2" r:id="rId3"/>
+    <sheet name="ASCII" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>VALOR</t>
   </si>
@@ -102,6 +103,12 @@
   </si>
   <si>
     <t>POSIÇÃO</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -262,6 +269,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -270,12 +283,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -439,8 +446,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CFBB581F-0D66-457B-BFC7-EE0705F9BF25}" name="ARRAY" displayName="ARRAY" ref="B8:C14" totalsRowShown="0">
-  <autoFilter ref="B8:C14" xr:uid="{C2684EE6-6435-4E57-82F4-8EFFA7BBA5EA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CFBB581F-0D66-457B-BFC7-EE0705F9BF25}" name="ARRAY" displayName="ARRAY" ref="A2:B8" totalsRowShown="0">
+  <autoFilter ref="A2:B8" xr:uid="{C2684EE6-6435-4E57-82F4-8EFFA7BBA5EA}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{6B7376DF-26A6-453D-85A8-B7DC1DAF78BC}" name="IND" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{982411CB-E3E1-4BE7-B53E-13C9A4232A94}" name="VALOR" dataDxfId="0"/>
@@ -843,10 +850,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A0DEAB-61BE-4E9E-890B-4E6A7C56F0DA}">
-  <dimension ref="B6:AL10"/>
+  <dimension ref="B6:AJ10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="AD10" sqref="AD10"/>
+    <sheetView showGridLines="0" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="AD13" sqref="AD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,42 +898,42 @@
     <col min="38" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:36" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="13" t="s">
+    <row r="6" spans="2:36" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="14">
-        <v>1</v>
-      </c>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="L6" s="14">
+      <c r="H6" s="11">
+        <v>1</v>
+      </c>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="L6" s="11">
         <v>2</v>
       </c>
-      <c r="M6" s="14"/>
-      <c r="P6" s="14">
+      <c r="M6" s="11"/>
+      <c r="P6" s="11">
         <v>3</v>
       </c>
-      <c r="Q6" s="14"/>
-      <c r="T6" s="14">
+      <c r="Q6" s="11"/>
+      <c r="T6" s="11">
         <v>4</v>
       </c>
-      <c r="U6" s="14"/>
-      <c r="X6" s="14">
+      <c r="U6" s="11"/>
+      <c r="X6" s="11">
         <v>5</v>
       </c>
-      <c r="Y6" s="14"/>
-      <c r="AB6" s="14">
+      <c r="Y6" s="11"/>
+      <c r="AB6" s="11">
         <v>6</v>
       </c>
-      <c r="AC6" s="14"/>
-      <c r="AG6" s="14"/>
-      <c r="AH6" s="14"/>
-      <c r="AI6" s="14"/>
+      <c r="AC6" s="11"/>
+      <c r="AG6" s="11"/>
+      <c r="AH6" s="11"/>
+      <c r="AI6" s="11"/>
     </row>
     <row r="7" spans="2:36" ht="2.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="12" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -981,7 +988,7 @@
       </c>
     </row>
     <row r="9" spans="2:36" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
+      <c r="B9" s="13"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
@@ -1000,7 +1007,7 @@
       <c r="AH9" s="6"/>
     </row>
     <row r="10" spans="2:36" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="12"/>
+      <c r="B10" s="14"/>
       <c r="D10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1049,80 +1056,77 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B36A3BB-8185-4C74-8FF9-A0084781F626}">
-  <dimension ref="B6:G14"/>
+  <dimension ref="A2:G8"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4">
+        <f>ARRAY!H10</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4">
+        <f>ARRAY!L10</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4">
+        <f>ARRAY!P10</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4">
+        <f>ARRAY!T10</f>
+        <v>4</v>
+      </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="6">
-        <v>0</v>
-      </c>
-      <c r="C9" s="4">
-        <f>ARRAY!H10</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="6">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4">
-        <f>ARRAY!L10</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
-        <v>2</v>
-      </c>
-      <c r="C11" s="4">
-        <f>ARRAY!P10</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="6">
-        <v>3</v>
-      </c>
-      <c r="C12" s="4">
-        <f>ARRAY!T10</f>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="6">
-        <v>4</v>
-      </c>
-      <c r="C13" s="4">
+      <c r="B7" s="4">
         <f>ARRAY!X10</f>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="6">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <v>5</v>
       </c>
-      <c r="C14" s="4">
+      <c r="B8" s="4">
         <f>ARRAY!AB10</f>
         <v>9</v>
       </c>
@@ -1133,4 +1137,187 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{805E168D-B08E-4478-8A20-3835D6774130}">
+  <dimension ref="A3:K10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>32</v>
+      </c>
+      <c r="H3">
+        <v>64</v>
+      </c>
+      <c r="I3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>128</v>
+      </c>
+      <c r="B8">
+        <v>64</v>
+      </c>
+      <c r="C8">
+        <v>32</v>
+      </c>
+      <c r="D8">
+        <v>16</v>
+      </c>
+      <c r="F8">
+        <v>8</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>65</v>
+      </c>
+      <c r="K9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>66</v>
+      </c>
+      <c r="K10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>